<commit_message>
Added excel sheet runtimes
</commit_message>
<xml_diff>
--- a/ExcelSheets/Runtimes.xlsx
+++ b/ExcelSheets/Runtimes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelscoleri/Desktop/Coding/School/Algos/cs330_transportation_networks/ExcelSheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F8C2F00-E018-1C4A-9DED-FF1FF61FFCB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C581D6C4-7C4C-FF4B-BFE7-54486DF126E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{F462E2C6-24DA-EB41-9EA2-A640277FB0E4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="9">
   <si>
     <t>n</t>
   </si>
@@ -54,6 +54,15 @@
   </si>
   <si>
     <t>OA (ms)</t>
+  </si>
+  <si>
+    <t>Edges</t>
+  </si>
+  <si>
+    <t>Dijkstra (ms)</t>
+  </si>
+  <si>
+    <t>Vertices</t>
   </si>
 </sst>
 </file>
@@ -377,6 +386,55 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Nodes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -439,6 +497,55 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Runtime (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -649,6 +756,36 @@
           <c:dLbls>
             <c:delete val="1"/>
           </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$10:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$B$10:$B$16</c:f>
@@ -715,6 +852,36 @@
           <c:dLbls>
             <c:delete val="1"/>
           </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$10:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$C$10:$C$16</c:f>
@@ -772,6 +939,55 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Nodes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -834,6 +1050,59 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="0E2841"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Runtime (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1235,6 +1504,55 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Nodes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -1297,6 +1615,59 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="0E2841"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Runtime (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1491,7 +1862,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$18</c:f>
+              <c:f>Sheet1!$B$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1698,6 +2069,60 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Nodes</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -1760,6 +2185,59 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="0E2841"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Runtime (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2161,6 +2639,55 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Nodes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -2223,6 +2750,59 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="0E2841"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Runtime (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2252,6 +2832,1055 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="117788512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Runtime</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> (ms) vs number of Edges</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$49</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dijkstra (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$50:$A$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3700</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>89000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>310000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>622000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>659000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$50:$B$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>339.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>522.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>760</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F999-404B-86E2-77B941689662}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$49</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> Contraction Hierarchies time (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$50:$A$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3700</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>89000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>310000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>622000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>659000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$50:$C$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F999-404B-86E2-77B941689662}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="291544848"/>
+        <c:axId val="282135568"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="291544848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Edges</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="282135568"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="282135568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Runtime (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="291544848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Runtime (ms) vs number of Vertices</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$49</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dijkstra (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$58:$A$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>214000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>449000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>513000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$50:$B$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>339.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>522.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>760</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9182-E74C-8D1E-8578F520E282}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$49</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> Contraction Hierarchies time (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$58:$A$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>214000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>449000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>513000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$50:$C$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9182-E74C-8D1E-8578F520E282}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="489343776"/>
+        <c:axId val="428802960"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="489343776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Vertices</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="428802960"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="428802960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Runtime (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="489343776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2520,6 +4149,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="231">
   <cs:axisTitle>
@@ -4393,6 +6102,942 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="231">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700">
+        <a:solidFill>
+          <a:schemeClr val="lt2"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="231">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700">
+        <a:solidFill>
+          <a:schemeClr val="lt2"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="231">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4938,16 +7583,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5015,15 +7660,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5045,6 +7690,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>933450</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CBCF088-BED7-366C-B9A4-C11E980F351C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>933450</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B66BD336-C3FC-764E-C01E-BDE87601317E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5370,16 +8087,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CEAC38E-DA0C-DE48-B6F9-6C7DCCD50A14}">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="L71" sqref="L71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
@@ -5860,6 +8577,102 @@
         <v>14.7</v>
       </c>
     </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>3700</v>
+      </c>
+      <c r="B50">
+        <v>2.4</v>
+      </c>
+      <c r="C50">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>89000</v>
+      </c>
+      <c r="B51">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="C51">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>310000</v>
+      </c>
+      <c r="B52">
+        <v>339.3</v>
+      </c>
+      <c r="C52">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>622000</v>
+      </c>
+      <c r="B53">
+        <v>522.9</v>
+      </c>
+      <c r="C53">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>659000</v>
+      </c>
+      <c r="B54">
+        <v>760</v>
+      </c>
+      <c r="C54">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>214000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>449000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>513000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>